<commit_message>
Daniel's test plan/procedure done
</commit_message>
<xml_diff>
--- a/Test Plans - HH2/test_procedure_Daniel.xlsx
+++ b/Test Plans - HH2/test_procedure_Daniel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="211">
   <si>
     <t>Reviewed by:</t>
   </si>
@@ -300,30 +300,6 @@
     <t>T_8</t>
   </si>
   <si>
-    <t>Compile single file source code</t>
-  </si>
-  <si>
-    <t>Compile multiple file source code</t>
-  </si>
-  <si>
-    <t>Fail compiling bad source code</t>
-  </si>
-  <si>
-    <t>Provide time limit verdict</t>
-  </si>
-  <si>
-    <t>Provide runtime exception verdict</t>
-  </si>
-  <si>
-    <t>Provide memory limit verdict</t>
-  </si>
-  <si>
-    <t>Provide wrong answer verdict</t>
-  </si>
-  <si>
-    <t>Provice correct answer verdict</t>
-  </si>
-  <si>
     <t>Create Assignment</t>
   </si>
   <si>
@@ -426,21 +402,6 @@
     <t>Status Code: 200, body contains user information along with its courses, assignments and submissions</t>
   </si>
   <si>
-    <t>Time Limit Exception</t>
-  </si>
-  <si>
-    <t>Memory Limit Exception</t>
-  </si>
-  <si>
-    <t>Runtime Exception</t>
-  </si>
-  <si>
-    <t>Wrong Answer</t>
-  </si>
-  <si>
-    <t>Correct Answer</t>
-  </si>
-  <si>
     <t>Status Code: 200, body contains assignment information</t>
   </si>
   <si>
@@ -573,9 +534,6 @@
     <t>:tid is replaced with the test case id</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>Daniel Santiago</t>
   </si>
   <si>
@@ -589,6 +547,111 @@
   </si>
   <si>
     <t>Browser (Chrome)</t>
+  </si>
+  <si>
+    <t>Single file correct verdict</t>
+  </si>
+  <si>
+    <t>Compile error verdict</t>
+  </si>
+  <si>
+    <t>I/O piping</t>
+  </si>
+  <si>
+    <t>Runtime Exception verdict</t>
+  </si>
+  <si>
+    <t>Single file wrong answer verdict</t>
+  </si>
+  <si>
+    <t>Multiple files correct verdict</t>
+  </si>
+  <si>
+    <t>Multiple files wrong answer verdict</t>
+  </si>
+  <si>
+    <t>T_9</t>
+  </si>
+  <si>
+    <t>T_10</t>
+  </si>
+  <si>
+    <t>Queue test</t>
+  </si>
+  <si>
+    <t>{ 'score': 10, 'timeLimit': 10, 'memLimit': 5 }</t>
+  </si>
+  <si>
+    <t>Multipart/form-data POST of files testInput.txt as testInput, testOutput.txt as testOutput, ExampleProgram.java as testerFile</t>
+  </si>
+  <si>
+    <t>Status Code: 200, body contains verdict: Correct</t>
+  </si>
+  <si>
+    <t>Status Code: 200, body contains verdict: Wrong Answer</t>
+  </si>
+  <si>
+    <t>Status Code: 200, body contains verdict: Compile Error</t>
+  </si>
+  <si>
+    <t>Status Code: 200, body contains verdict: Runtime Exception</t>
+  </si>
+  <si>
+    <t>Go to ./jsubmit.html. Select ExampleProgram.java as source file. Expected Output field should be: "I'm a Simple Program."</t>
+  </si>
+  <si>
+    <t>Files are located in panda/test/res</t>
+  </si>
+  <si>
+    <t>Go to ./jsubmit.html. Select ExampleProgram.java as source file. Expected Output field should be left empty.</t>
+  </si>
+  <si>
+    <t>Go to ./jsubmit.html. Select BadExampleProgram.java as source file.</t>
+  </si>
+  <si>
+    <t>Go to ./jsubmit.html. Select ReadInput.java as source file. Input field must be "Hola Mundo" and Expected Output field must be "Hola Mundo".</t>
+  </si>
+  <si>
+    <t>Providing same input and output confirms that the programs receives input from standard I/O streams</t>
+  </si>
+  <si>
+    <t>Go to ./jsubmit.html. Select RuntimeEx.java as source file.</t>
+  </si>
+  <si>
+    <t>Go to ./jsubmit.html. Select InfiniteLoop.java as source file.</t>
+  </si>
+  <si>
+    <t>Status Code: 200, body contains verdict: Time Limit Exceeded</t>
+  </si>
+  <si>
+    <t>Time limit exceeded verdict</t>
+  </si>
+  <si>
+    <t>Memory limit exceeded verdict</t>
+  </si>
+  <si>
+    <t>Status Code: 200, body contains verdict: Memory Limit Exceeded</t>
+  </si>
+  <si>
+    <t>3 seconds time limit</t>
+  </si>
+  <si>
+    <t>Go to ./jsubmit.html. Select MemO.java as source file.</t>
+  </si>
+  <si>
+    <t>~25Mb memory limit</t>
+  </si>
+  <si>
+    <t>Go to ./zipsubmit.html. Select source archive llzip.zip as source file. Select IndexListTester.java as Main Class Tester. Expected Output must be equal to the contents of llReferenceOutput.txt</t>
+  </si>
+  <si>
+    <t>Go to ./zipsubmit.html. Select source archive llzip.zip as source file. Select IndexListTester.java as Main Class Tester. Expected Output must be empty</t>
+  </si>
+  <si>
+    <t>Perform HTTP GET to ./test/queue. Watch console.</t>
+  </si>
+  <si>
+    <t>Internal workflow of a queue is processed grading a multiple file source code with multiple tests.</t>
   </si>
 </sst>
 </file>
@@ -794,7 +857,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -827,51 +890,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -910,6 +931,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -917,40 +977,6 @@
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD8D8D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -996,6 +1022,23 @@
         <bottom/>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1058,13 +1101,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1078,6 +1114,30 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFD8D8D8"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1093,15 +1153,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A18:G67" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3" headerRowBorderDxfId="9" tableBorderDxfId="10">
-  <autoFilter ref="A18:G67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A18:G69" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
+  <autoFilter ref="A18:G69"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Test ID" dataDxfId="8"/>
-    <tableColumn id="2" name="Test Description" dataDxfId="7"/>
-    <tableColumn id="3" name="Instructions" dataDxfId="6"/>
-    <tableColumn id="7" name="Payload" dataDxfId="1"/>
-    <tableColumn id="4" name="Expected Outcome" dataDxfId="5"/>
-    <tableColumn id="5" name="Pass/Fail" dataDxfId="4"/>
+    <tableColumn id="1" name="Test ID" dataDxfId="6"/>
+    <tableColumn id="2" name="Test Description" dataDxfId="5"/>
+    <tableColumn id="3" name="Instructions" dataDxfId="4"/>
+    <tableColumn id="7" name="Payload" dataDxfId="3"/>
+    <tableColumn id="4" name="Expected Outcome" dataDxfId="2"/>
+    <tableColumn id="5" name="Pass/Fail" dataDxfId="1"/>
     <tableColumn id="6" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1371,10 +1431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,10 +1442,10 @@
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" style="16" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" style="35" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1401,7 +1461,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1417,7 +1477,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1436,1117 +1496,1189 @@
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="E7" s="17" t="s">
+      <c r="B7" s="32"/>
+      <c r="E7" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="E8" s="19" t="s">
+      <c r="B8" s="29"/>
+      <c r="E8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22"/>
+      <c r="B9" s="29"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="E10" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="F10" s="24"/>
+      <c r="B10" s="29"/>
+      <c r="E10" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="13"/>
+      <c r="B11" s="29"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="B12" s="13"/>
+      <c r="A12" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="29"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="B13" s="13"/>
+      <c r="A13" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="29"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="B14" s="13"/>
+      <c r="A14" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="29"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="29"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="31"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" s="26" t="s">
+      <c r="D18" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="22" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D19" s="41" t="s">
-        <v>172</v>
+        <v>134</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>159</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F19" s="5">
         <v>1</v>
       </c>
-      <c r="G19" s="34" t="s">
-        <v>173</v>
+      <c r="G19" s="20" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>149</v>
+        <v>134</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F20" s="6">
         <v>1</v>
       </c>
-      <c r="G20" s="37"/>
+      <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>149</v>
+        <v>138</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F21" s="6">
         <v>1</v>
       </c>
-      <c r="G21" s="37" t="s">
-        <v>170</v>
+      <c r="G21" s="23" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>149</v>
+        <v>135</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F22" s="6">
         <v>1</v>
       </c>
-      <c r="G22" s="37"/>
+      <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>149</v>
+        <v>139</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F23" s="6">
         <v>1</v>
       </c>
-      <c r="G23" s="37"/>
+      <c r="G23" s="23"/>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>149</v>
+        <v>140</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F24" s="6">
         <v>1</v>
       </c>
-      <c r="G24" s="37" t="s">
-        <v>171</v>
+      <c r="G24" s="23" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>149</v>
+        <v>138</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F25" s="6">
         <v>1</v>
       </c>
-      <c r="G25" s="37"/>
+      <c r="G25" s="23"/>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>149</v>
+        <v>140</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F26" s="6">
         <v>1</v>
       </c>
-      <c r="G26" s="37"/>
+      <c r="G26" s="23"/>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>149</v>
+        <v>140</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F27" s="6">
         <v>1</v>
       </c>
-      <c r="G27" s="37"/>
+      <c r="G27" s="23"/>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>47</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>149</v>
+        <v>141</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F28" s="6">
         <v>1</v>
       </c>
-      <c r="G28" s="37"/>
+      <c r="G28" s="23"/>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>149</v>
+        <v>141</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F29" s="6">
         <v>1</v>
       </c>
-      <c r="G29" s="37"/>
+      <c r="G29" s="23"/>
     </row>
     <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>149</v>
+        <v>138</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F30" s="6">
         <v>1</v>
       </c>
-      <c r="G30" s="37"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>149</v>
+        <v>142</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F31" s="6">
         <v>1</v>
       </c>
-      <c r="G31" s="37"/>
+      <c r="G31" s="23"/>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>149</v>
+        <v>142</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F32" s="6">
         <v>1</v>
       </c>
-      <c r="G32" s="37"/>
+      <c r="G32" s="23"/>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D33" s="32" t="s">
-        <v>149</v>
+        <v>138</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>136</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F33" s="7">
         <v>1</v>
       </c>
-      <c r="G33" s="38"/>
+      <c r="G33" s="24"/>
     </row>
     <row r="34" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="12" t="s">
         <v>53</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>71</v>
       </c>
       <c r="C34" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>169</v>
-      </c>
       <c r="E34" s="9" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F34" s="6">
         <v>1</v>
       </c>
-      <c r="G34" s="34" t="s">
-        <v>174</v>
+      <c r="G34" s="20" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>72</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>149</v>
+        <v>143</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F35" s="6">
         <v>1</v>
       </c>
-      <c r="G35" s="37"/>
+      <c r="G35" s="23"/>
     </row>
     <row r="36" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>73</v>
       </c>
       <c r="C36" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="D36" s="41" t="s">
-        <v>169</v>
-      </c>
       <c r="E36" s="9" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F36" s="6">
         <v>1</v>
       </c>
-      <c r="G36" s="39"/>
+      <c r="G36" s="25"/>
     </row>
     <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>74</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="D37" s="41" t="s">
-        <v>176</v>
+        <v>144</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>163</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F37" s="6">
         <v>1</v>
       </c>
-      <c r="G37" s="40"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="D38" s="41" t="s">
-        <v>177</v>
+        <v>144</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>164</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F38" s="6">
         <v>1</v>
       </c>
-      <c r="G38" s="40"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="12" t="s">
         <v>58</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="D39" s="41" t="s">
-        <v>175</v>
+        <v>144</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>162</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F39" s="6">
         <v>1</v>
       </c>
-      <c r="G39" s="40"/>
+      <c r="G39" s="26"/>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>77</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>149</v>
+        <v>146</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F40" s="6">
         <v>1</v>
       </c>
-      <c r="G40" s="40" t="s">
-        <v>178</v>
+      <c r="G40" s="26" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>78</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>149</v>
+        <v>145</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F41" s="6">
         <v>1</v>
       </c>
-      <c r="G41" s="40"/>
+      <c r="G41" s="26"/>
     </row>
     <row r="42" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="12" t="s">
         <v>61</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>79</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F42" s="6">
         <v>1</v>
       </c>
-      <c r="G42" s="40"/>
+      <c r="G42" s="26"/>
     </row>
     <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="12" t="s">
         <v>83</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>80</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F43" s="6">
         <v>1</v>
       </c>
-      <c r="G43" s="40"/>
+      <c r="G43" s="26"/>
     </row>
     <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="12" t="s">
         <v>84</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>81</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D44" s="29" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F44" s="6">
         <v>1</v>
       </c>
-      <c r="G44" s="40"/>
+      <c r="G44" s="26"/>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="12" t="s">
         <v>85</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>82</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="D45" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" s="6">
+        <v>1</v>
+      </c>
+      <c r="G45" s="24"/>
+    </row>
+    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F46" s="6">
+        <v>1</v>
+      </c>
+      <c r="G46" s="24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D47" s="15"/>
+      <c r="E47" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="F47" s="6">
+        <v>1</v>
+      </c>
+      <c r="G47" s="24"/>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D48" s="18"/>
+      <c r="E48" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F48" s="6">
+        <v>1</v>
+      </c>
+      <c r="G48" s="24"/>
+    </row>
+    <row r="49" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D49" s="18"/>
+      <c r="E49" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F49" s="6">
+        <v>1</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D50" s="18"/>
+      <c r="E50" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F50" s="6">
+        <v>1</v>
+      </c>
+      <c r="G50" s="24"/>
+    </row>
+    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D51" s="18"/>
+      <c r="E51" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F51" s="6">
+        <v>1</v>
+      </c>
+      <c r="G51" s="24" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" s="18"/>
+      <c r="E52" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F52" s="6">
+        <v>1</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D53" s="15"/>
+      <c r="E53" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F53" s="6">
+        <v>1</v>
+      </c>
+      <c r="G53" s="24"/>
+    </row>
+    <row r="54" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D54" s="15"/>
+      <c r="E54" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="F54" s="6">
+        <v>1</v>
+      </c>
+      <c r="G54" s="24"/>
+    </row>
+    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D55" s="18"/>
+      <c r="E55" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F55" s="6">
+        <v>1</v>
+      </c>
+      <c r="G55" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E45" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F45" s="6">
-        <v>1</v>
-      </c>
-      <c r="G45" s="38"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="6">
-        <v>1</v>
-      </c>
-      <c r="G46" s="38"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="10" t="s">
+      <c r="D56" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F56" s="6">
+        <v>1</v>
+      </c>
+      <c r="G56" s="20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="6">
-        <v>1</v>
-      </c>
-      <c r="G47" s="38"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="B48" s="10" t="s">
+      <c r="C57" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F57" s="6">
+        <v>1</v>
+      </c>
+      <c r="G57" s="26"/>
+    </row>
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="6">
-        <v>1</v>
-      </c>
-      <c r="G48" s="38"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="10" t="s">
+      <c r="C58" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F58" s="6">
+        <v>1</v>
+      </c>
+      <c r="G58" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="F49" s="6">
-        <v>1</v>
-      </c>
-      <c r="G49" s="38"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="10" t="s">
+      <c r="C59" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F59" s="6">
+        <v>1</v>
+      </c>
+      <c r="G59" s="26"/>
+    </row>
+    <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F50" s="6">
-        <v>1</v>
-      </c>
-      <c r="G50" s="38"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="B51" s="10" t="s">
+      <c r="C60" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F60" s="6">
+        <v>1</v>
+      </c>
+      <c r="G60" s="26"/>
+    </row>
+    <row r="61" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C51" s="10"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="F51" s="6">
-        <v>1</v>
-      </c>
-      <c r="G51" s="38"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" s="10" t="s">
+      <c r="C61" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F61" s="6">
+        <v>1</v>
+      </c>
+      <c r="G61" s="26"/>
+    </row>
+    <row r="62" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B62" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="10"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F52" s="6">
-        <v>1</v>
-      </c>
-      <c r="G52" s="38"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="B53" s="10" t="s">
+      <c r="C62" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F62" s="6">
+        <v>1</v>
+      </c>
+      <c r="G62" s="26"/>
+    </row>
+    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C53" s="10"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F53" s="7">
-        <v>1</v>
-      </c>
-      <c r="G53" s="38"/>
-    </row>
-    <row r="54" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B54" s="9" t="s">
+      <c r="B63" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F63" s="6">
+        <v>1</v>
+      </c>
+      <c r="G63" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="D54" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F54" s="6">
-        <v>1</v>
-      </c>
-      <c r="G54" s="34" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" s="9" t="s">
+      <c r="B64" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F64" s="6">
+        <v>1</v>
+      </c>
+      <c r="G64" s="26"/>
+    </row>
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="D55" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F55" s="6">
-        <v>1</v>
-      </c>
-      <c r="G55" s="40"/>
-    </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B56" s="9" t="s">
+      <c r="B65" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F65" s="6">
+        <v>1</v>
+      </c>
+      <c r="G65" s="26"/>
+    </row>
+    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A66" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C56" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D56" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="F56" s="6">
-        <v>1</v>
-      </c>
-      <c r="G56" s="40" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="B57" s="9" t="s">
+      <c r="B66" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D66" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F66" s="6">
+        <v>1</v>
+      </c>
+      <c r="G66" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D57" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F57" s="6">
-        <v>1</v>
-      </c>
-      <c r="G57" s="40"/>
-    </row>
-    <row r="58" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B58" s="9" t="s">
+      <c r="B67" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F67" s="6">
+        <v>1</v>
+      </c>
+      <c r="G67" s="26"/>
+    </row>
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C58" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D58" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="F58" s="6">
-        <v>1</v>
-      </c>
-      <c r="G58" s="40"/>
-    </row>
-    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B59" s="9" t="s">
+      <c r="B68" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F68" s="6">
+        <v>1</v>
+      </c>
+      <c r="G68" s="26"/>
+    </row>
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D59" s="41" t="s">
-        <v>182</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F59" s="6">
-        <v>1</v>
-      </c>
-      <c r="G59" s="40"/>
-    </row>
-    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D60" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F60" s="6">
-        <v>1</v>
-      </c>
-      <c r="G60" s="40"/>
-    </row>
-    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D61" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F61" s="6">
-        <v>1</v>
-      </c>
-      <c r="G61" s="40" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D62" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="F62" s="6">
-        <v>1</v>
-      </c>
-      <c r="G62" s="40"/>
-    </row>
-    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D63" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F63" s="6">
-        <v>1</v>
-      </c>
-      <c r="G63" s="40"/>
-    </row>
-    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D64" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F64" s="6">
-        <v>1</v>
-      </c>
-      <c r="G64" s="40" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="25" t="s">
+      <c r="B69" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B65" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="D65" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F65" s="6">
-        <v>1</v>
-      </c>
-      <c r="G65" s="40"/>
-    </row>
-    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="D66" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="F66" s="6">
-        <v>1</v>
-      </c>
-      <c r="G66" s="40"/>
-    </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
+      <c r="C69" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B67" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D67" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F67" s="28">
-        <v>1</v>
-      </c>
-      <c r="G67" s="39"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E68" t="s">
+      <c r="F69" s="6">
+        <v>1</v>
+      </c>
+      <c r="G69" s="25"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
         <v>70</v>
       </c>
-      <c r="F68">
-        <f>((COUNTIF(F19:F67,"1")/COUNT(F19:F67))*100)</f>
+      <c r="F70">
+        <f>((COUNTIF(F19:F69,"1")/COUNT(F19:F69))*100)</f>
         <v>100</v>
       </c>
     </row>
@@ -2566,7 +2698,16 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
   </mergeCells>
-  <conditionalFormatting sqref="F19:F67">
+  <conditionalFormatting sqref="F19:F54 F56:F69">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F55">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>

</xml_diff>